<commit_message>
commiting git tracker files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Signup" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="LoginData" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Dashboard" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="EditYourProfile" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -19,14 +19,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>testvaliduser@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>wrong@gmail.com</t>
+  </si>
+  <si>
+    <t>wrong123</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -46,9 +82,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -292,13 +331,50 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="26.71"/>
+    <col customWidth="1" min="2" max="2" width="29.43"/>
+    <col customWidth="1" min="3" max="3" width="21.0"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
working on Onboarding Scenarios  Step 3  UI verifcation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Signup" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Login" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="LoginData" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Dashboard" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="EditYourProfile" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -19,14 +19,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>testvaliduser@gmail.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>wrong@gmail.com</t>
+  </si>
+  <si>
+    <t>wrong123</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -46,9 +82,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -292,13 +331,50 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="26.71"/>
+    <col customWidth="1" min="2" max="2" width="29.43"/>
+    <col customWidth="1" min="3" max="3" width="21.0"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated Onboarding3FnStep feature, step def and pages
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -4,22 +4,25 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Signup" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="LoginData" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Dashboard" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="EditYourProfile" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="OnBoardingStep7" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet7" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="LoginData" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Dashboard" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="EditYourProfile" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="OnBoarding" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="Jl0lNtklzwoVo8e5XLCuQG5Dq9Aqocp3z/4gMZuF1uQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -96,6 +99,24 @@
     </r>
   </si>
   <si>
+    <t>validweight</t>
+  </si>
+  <si>
+    <t>validheight</t>
+  </si>
+  <si>
+    <t>Invalidweight</t>
+  </si>
+  <si>
+    <t>Invalidheight</t>
+  </si>
+  <si>
+    <t>validDate</t>
+  </si>
+  <si>
+    <t>InvalidDate</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -115,13 +136,144 @@
   </si>
   <si>
     <t>blank</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>With Report/Without Report</t>
+  </si>
+  <si>
+    <t>Health Conditions</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>BP Status</t>
+  </si>
+  <si>
+    <t>Menstrual Cycle Track</t>
+  </si>
+  <si>
+    <t>Last Period Date</t>
+  </si>
+  <si>
+    <t>Weight in KG</t>
+  </si>
+  <si>
+    <t>Height in CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dietary Preferences
+</t>
+  </si>
+  <si>
+    <t>Physical Activity Level</t>
+  </si>
+  <si>
+    <t>Food Allergies
+&amp; Sensitivities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please select any foods you need to avoid:
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medications &amp; Supplements
+</t>
+  </si>
+  <si>
+    <t>select or add the medications/supplements you're taking</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>User1@gmail.com</t>
+  </si>
+  <si>
+    <t>User1@987&amp;</t>
+  </si>
+  <si>
+    <t>without report</t>
+  </si>
+  <si>
+    <t>Pre-diabetes / Diabetes , Hypothyroidism</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>I have been diagnosed but don't take medication</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Non-Vegetarian</t>
+  </si>
+  <si>
+    <t>Lightly Active</t>
+  </si>
+  <si>
+    <t>Yes, I have food intolerances/sensitivities</t>
+  </si>
+  <si>
+    <t>Fish, Peanuts</t>
+  </si>
+  <si>
+    <t>Yes, I take prescription medications</t>
+  </si>
+  <si>
+    <t>Thyroid medication,
+Vitamin D, Insulin</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>User2@gmail.com</t>
+  </si>
+  <si>
+    <t>User2*/245</t>
+  </si>
+  <si>
+    <t>PCOS</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>I'm not sure</t>
+  </si>
+  <si>
+    <t>My cycle is irregular</t>
+  </si>
+  <si>
+    <t>Vegetarian Diet</t>
+  </si>
+  <si>
+    <t>Sedentary</t>
+  </si>
+  <si>
+    <t>No, I can eat everything</t>
+  </si>
+  <si>
+    <t>No, I don't take any medications or supplements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -143,22 +295,57 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -170,6 +357,33 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -192,6 +406,18 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -504,6 +730,69 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5">
+        <v>34.0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>170.0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-4.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -519,7 +808,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -530,10 +819,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -541,18 +830,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1559,7 +1848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1573,7 +1862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1585,4 +1874,207 @@
   <sheetData/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="9">
+        <v>43.0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="10">
+        <v>46031.0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>67.0</v>
+      </c>
+      <c r="K2" s="9">
+        <v>145.0</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="9">
+        <v>25.0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="10">
+        <v>46054.0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>56.0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>160.0</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
loginUI validatins and condinal hooks
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -5,23 +5,24 @@
   <sheets>
     <sheet state="visible" name="Signup" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="OnBoardingStep7" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="LoginData" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Dashboard" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="EditYourProfile" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="OnBoarding" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Sheet7" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="LoginData" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Dashboard" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="EditYourProfile" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="OnBoarding" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="MaEq6S7PTP2Bt2XDlMZdddt9myVPUHHckoLvOPXqc68="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -110,6 +111,12 @@
     <t>Invalidheight</t>
   </si>
   <si>
+    <t>validDate</t>
+  </si>
+  <si>
+    <t>InvalidDate</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -263,10 +270,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -293,6 +301,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="&quot;Menlo&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -304,12 +317,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -338,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -357,25 +376,31 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -407,6 +432,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -739,6 +768,12 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5">
@@ -752,6 +787,12 @@
       </c>
       <c r="D2" s="5">
         <v>-4.0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45702.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>45143.0</v>
       </c>
     </row>
   </sheetData>
@@ -760,6 +801,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -777,7 +832,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -788,10 +843,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -799,18 +854,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1817,20 +1872,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -1854,194 +1895,208 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="M1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="O1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="P1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="Q1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="9">
+      <c r="D2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="11">
         <v>43.0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="G2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="12">
         <v>46031.0</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="11">
         <v>67.0</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="11">
         <v>145.0</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="L2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="M2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="O2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="P2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
+      <c r="Q2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="11">
+        <v>25.0</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="12">
+        <v>46054.0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>56.0</v>
+      </c>
+      <c r="K3" s="11">
+        <v>160.0</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="14"/>
+      <c r="P3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="9">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="10">
-        <v>46054.0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>56.0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
completed edit your profile module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -5,23 +5,24 @@
   <sheets>
     <sheet state="visible" name="Signup" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="OnBoardingStep7" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="LoginData" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Dashboard" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="EditYourProfile" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="OnBoarding" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Sheet7" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="LoginData" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Dashboard" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="EditYourProfile" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="OnBoarding" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="MaEq6S7PTP2Bt2XDlMZdddt9myVPUHHckoLvOPXqc68="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -110,6 +111,12 @@
     <t>Invalidheight</t>
   </si>
   <si>
+    <t>validDate</t>
+  </si>
+  <si>
+    <t>InvalidDate</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -129,6 +136,15 @@
   </si>
   <si>
     <t>blank</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>AlertText</t>
+  </si>
+  <si>
+    <t>Thyroid</t>
   </si>
   <si>
     <t>UserName</t>
@@ -263,10 +279,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -293,6 +310,16 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="&quot;Menlo&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -304,12 +331,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -338,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -351,31 +384,40 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -407,6 +449,10 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -739,19 +785,31 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>34.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>170.0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>0.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>-4.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>46036.0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>45143.0</v>
       </c>
     </row>
   </sheetData>
@@ -760,6 +818,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <pageSetUpPr/>
@@ -777,7 +849,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -788,10 +860,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -799,18 +871,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1817,20 +1889,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -1856,192 +1914,223 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="9">
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="12">
         <v>43.0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="G2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="13">
         <v>46031.0</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="12">
         <v>67.0</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="12">
         <v>145.0</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="L2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="M2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
+      <c r="N2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="A3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="12">
         <v>25.0</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="13">
+        <v>46054.0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>56.0</v>
+      </c>
+      <c r="K3" s="12">
+        <v>160.0</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="10">
-        <v>46054.0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>56.0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Completed onboarding step 4 functionality and 5 UI verification
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="t4f85315oZeYzB3iR8O3SlURAbhmYgzYUSDhuhPWuK8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -138,6 +138,15 @@
     <t>blank</t>
   </si>
   <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>AlertText</t>
+  </si>
+  <si>
+    <t>Thyroid</t>
+  </si>
+  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -191,6 +200,9 @@
   </si>
   <si>
     <t>Plan</t>
+  </si>
+  <si>
+    <t>User_WithoutReport</t>
   </si>
   <si>
     <t>User1@gmail.com</t>
@@ -270,10 +282,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -300,6 +313,16 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="&quot;Menlo&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -311,12 +334,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -345,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -358,31 +387,49 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -750,25 +797,31 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>34.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>170.0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>0.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>-4.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>46036.0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>45143.0</v>
       </c>
     </row>
   </sheetData>
@@ -1871,7 +1924,24 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1887,192 +1957,199 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="Q1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="9">
+      <c r="C2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="14">
         <v>43.0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="10">
+      <c r="H2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="15">
         <v>46031.0</v>
       </c>
-      <c r="J2" s="9">
+      <c r="K2" s="14">
         <v>67.0</v>
       </c>
-      <c r="K2" s="9">
+      <c r="L2" s="14">
         <v>145.0</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="8" t="s">
+      <c r="M2" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="N2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="O2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
+      <c r="P2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="14">
+        <v>25.0</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="15">
+        <v>46054.0</v>
+      </c>
+      <c r="K3" s="14">
+        <v>56.0</v>
+      </c>
+      <c r="L3" s="14">
+        <v>160.0</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="18"/>
+      <c r="S3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="9">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="10">
-        <v>46054.0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>56.0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Commmint latest menstrual log changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="t4f85315oZeYzB3iR8O3SlURAbhmYgzYUSDhuhPWuK8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -138,6 +138,15 @@
     <t>blank</t>
   </si>
   <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>AlertText</t>
+  </si>
+  <si>
+    <t>Thyroid</t>
+  </si>
+  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -193,6 +202,9 @@
     <t>Plan</t>
   </si>
   <si>
+    <t>User_WithoutReport</t>
+  </si>
+  <si>
     <t>User1@gmail.com</t>
   </si>
   <si>
@@ -233,47 +245,73 @@
 Vitamin D, Insulin</t>
   </si>
   <si>
+    <t>Free Plan</t>
+  </si>
+  <si>
+    <t>User2@gmail.com</t>
+  </si>
+  <si>
+    <t>User2*/245</t>
+  </si>
+  <si>
+    <t>PCOS</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>I'm not sure</t>
+  </si>
+  <si>
+    <t>My cycle is irregular</t>
+  </si>
+  <si>
+    <t>Vegetarian Diet</t>
+  </si>
+  <si>
+    <t>Sedentary</t>
+  </si>
+  <si>
+    <t>No, I can eat everything</t>
+  </si>
+  <si>
+    <t>No, I don't take any medications or supplements</t>
+  </si>
+  <si>
     <t>Free</t>
   </si>
   <si>
-    <t>User2@gmail.com</t>
-  </si>
-  <si>
-    <t>User2*/245</t>
-  </si>
-  <si>
-    <t>PCOS</t>
-  </si>
-  <si>
-    <t>User2</t>
-  </si>
-  <si>
-    <t>I'm not sure</t>
-  </si>
-  <si>
-    <t>My cycle is irregular</t>
-  </si>
-  <si>
-    <t>Vegetarian Diet</t>
-  </si>
-  <si>
-    <t>Sedentary</t>
-  </si>
-  <si>
-    <t>No, I can eat everything</t>
-  </si>
-  <si>
-    <t>No, I don't take any medications or supplements</t>
+    <t>User_WithoutReport_WithOnlyHealthCondition</t>
+  </si>
+  <si>
+    <t>gurdev@gmail.com</t>
+  </si>
+  <si>
+    <t>Success@1</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>gurdev</t>
+  </si>
+  <si>
+    <t>I have never been diagnosed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Non-Vegetarian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -300,6 +338,16 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="&quot;Menlo&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -311,12 +359,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -345,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -358,32 +412,59 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,25 +831,31 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>34.0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>170.0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>0.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>-4.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>46036.0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>45143.0</v>
       </c>
     </row>
   </sheetData>
@@ -1871,7 +1958,24 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1887,192 +1991,3240 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="Q1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="9">
+      <c r="C2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="14">
         <v>43.0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="15">
+        <v>46031.0</v>
+      </c>
+      <c r="K2" s="14">
+        <v>67.0</v>
+      </c>
+      <c r="L2" s="14">
+        <v>145.0</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="10">
-        <v>46031.0</v>
-      </c>
-      <c r="J2" s="9">
-        <v>67.0</v>
-      </c>
-      <c r="K2" s="9">
-        <v>145.0</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="E3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="14">
+        <v>25.0</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="15">
+        <v>46054.0</v>
+      </c>
+      <c r="K3" s="14">
+        <v>56.0</v>
+      </c>
+      <c r="L3" s="14">
+        <v>160.0</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="18"/>
+      <c r="S3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="J4" s="20">
+        <v>46036.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>155.0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="O4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="9">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="10">
-        <v>46054.0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>56.0</v>
-      </c>
-      <c r="K3" s="9">
-        <v>160.0</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="21"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="21"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="21"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="21"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="21"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="21"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="21"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="21"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="21"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="21"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="21"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="21"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="21"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="21"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="21"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="21"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="21"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="21"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="21"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="21"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="21"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="21"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="21"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="21"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="21"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="21"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="21"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="21"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="21"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="21"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="21"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="21"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="21"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="21"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="21"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="21"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="21"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="21"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="21"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="21"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="21"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="21"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="21"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="21"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="21"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="21"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="21"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="21"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="21"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="21"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="21"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="21"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="21"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="21"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="21"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="21"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="21"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="21"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="21"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="21"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="21"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="21"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="21"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="21"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="21"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="21"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="21"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="21"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="21"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="21"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="21"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="21"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="21"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="21"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="21"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="21"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="21"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="21"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="21"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="21"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="21"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="21"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="21"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="21"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="21"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="21"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="21"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="21"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="21"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="21"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="21"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="21"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="21"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="21"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="21"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="21"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="21"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="21"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="21"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="21"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="21"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="21"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="21"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="21"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="21"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="21"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="21"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="21"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="21"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="21"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="21"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="21"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="21"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="21"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="21"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="21"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="21"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="21"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="21"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="21"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="21"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="21"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="21"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="21"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="21"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="21"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="21"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="21"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="21"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="21"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="21"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="21"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="21"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="21"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="21"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="21"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="21"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="21"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="21"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="21"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="21"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="21"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="21"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="21"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="21"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="21"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="21"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="21"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="21"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="21"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="21"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="21"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="21"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="21"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="21"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="21"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="21"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="21"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="21"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="21"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="21"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="21"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="21"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="21"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="21"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="21"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="21"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="21"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="21"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="21"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="21"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="21"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="21"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="21"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="21"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="21"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="21"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="21"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="21"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="21"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="21"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="21"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="21"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="21"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="21"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="21"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="21"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="21"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="21"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="21"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="21"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="21"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="21"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="21"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="21"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="21"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="21"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="21"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="21"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="21"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="21"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="21"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="21"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="21"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="21"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="21"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="21"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="21"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="21"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="21"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="21"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="21"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="21"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="21"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="21"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="21"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="21"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="21"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="21"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="21"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="21"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="21"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="21"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="21"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="21"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="21"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="21"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="21"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="21"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="21"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="21"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="21"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="21"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="21"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="21"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="21"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="21"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="21"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="21"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="21"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="21"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="21"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="21"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="21"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="21"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="21"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="21"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="21"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="21"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="21"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="21"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="21"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="21"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="21"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="21"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="21"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="21"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="21"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="21"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="21"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="21"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="21"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="21"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="21"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="21"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="21"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="21"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="21"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="21"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="21"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="21"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="21"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="21"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="21"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="21"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="21"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="21"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="21"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="21"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="21"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="21"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="21"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="21"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="21"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="21"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="21"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="21"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="21"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="21"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="21"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="21"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="21"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="21"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="21"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="21"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="21"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="21"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="21"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="21"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="21"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="21"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="21"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="21"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="21"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="21"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="21"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="21"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="21"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="21"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="21"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="21"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="21"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="21"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="21"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="21"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="21"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="21"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="21"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="21"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="21"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="21"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="21"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="21"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="21"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="21"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="21"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="21"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="21"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="21"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="21"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="21"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="21"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="21"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="21"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="21"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="21"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="21"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="21"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="21"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="21"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="21"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="21"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="21"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="21"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="21"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="21"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="21"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="21"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="21"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="21"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="21"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="21"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="21"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="21"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="21"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="21"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="21"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="21"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="21"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="21"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="21"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="21"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="21"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="21"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="21"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="21"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="21"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="21"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="21"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="21"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="21"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="21"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="21"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="21"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="21"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="21"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="21"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="21"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="21"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="21"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="21"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="21"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="21"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="21"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="21"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="21"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="21"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="21"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="21"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="21"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="21"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="21"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="21"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="21"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="21"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="21"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="21"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="21"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="21"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="21"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="21"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="21"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="21"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="21"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="21"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="21"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="21"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="21"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="21"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="21"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="21"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="21"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="21"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="21"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="21"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="21"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="21"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="21"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="21"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="21"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="21"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="21"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="21"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="21"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="21"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="21"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="21"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="21"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="21"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="21"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="21"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="21"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="21"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="21"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="21"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="21"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="21"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="21"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="21"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="21"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="21"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="21"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="21"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="21"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="21"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="21"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="21"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="21"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="21"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="21"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="21"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="21"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="21"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="21"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="21"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="21"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="21"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="21"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="21"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="21"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="21"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="21"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="21"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="21"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="21"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="21"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="21"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="21"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="21"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="21"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="21"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="21"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="21"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="21"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="21"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="21"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="21"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="21"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="21"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="21"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="21"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="21"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="21"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="21"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="21"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="21"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="21"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="21"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="21"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="21"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="21"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="21"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="21"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="21"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="21"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="21"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="21"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="21"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="21"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="21"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="21"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="21"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="21"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="21"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="21"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="21"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="21"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="21"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="21"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="21"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="21"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="21"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="21"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="21"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="21"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="21"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="21"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="21"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="21"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="21"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="21"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="21"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="21"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="21"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="21"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="21"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="21"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="21"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="21"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="21"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="21"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="21"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="21"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="21"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="21"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="21"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="21"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="21"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="21"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="21"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="21"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="21"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="21"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="21"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="21"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="21"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="21"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="21"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="21"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="21"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="21"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="21"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="21"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="21"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="21"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="21"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="21"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="21"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="21"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="21"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="21"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="21"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="21"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="21"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="21"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="21"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="21"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="21"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="21"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="21"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="21"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="21"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="21"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="21"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="21"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="21"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="21"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="21"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="21"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="21"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="21"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="21"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="21"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="21"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="21"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="21"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="21"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="21"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="21"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="21"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="21"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="21"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="21"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="21"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="21"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="21"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="21"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="21"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="21"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="21"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="21"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="21"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="21"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="21"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="21"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="21"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="21"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="21"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="21"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="21"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="21"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="21"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="21"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="21"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="21"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="21"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="21"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="21"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="21"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="21"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="21"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="21"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="21"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="21"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="21"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="21"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="21"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="21"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="21"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="21"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="21"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="21"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="21"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="21"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="21"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="21"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="21"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="21"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="21"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="21"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="21"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="21"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="21"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="21"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="21"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="21"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="21"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="21"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="21"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="21"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="21"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="21"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="21"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="21"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="21"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="21"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="21"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="21"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="21"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="21"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="21"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="21"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="21"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="21"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="21"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="21"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="21"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="21"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="21"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="21"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="21"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="21"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="21"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="21"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="21"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="21"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="21"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="21"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="21"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="21"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="21"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="21"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="21"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="21"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="21"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="21"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="21"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="21"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="21"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="21"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="21"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="21"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="21"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="21"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="21"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="21"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="21"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="21"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="21"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="21"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="21"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="21"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="21"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="21"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="21"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="21"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="21"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="21"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="21"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="21"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="21"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="21"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="21"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="21"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="21"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="21"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="21"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="21"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="21"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="21"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="21"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="21"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="21"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="21"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="21"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="21"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="21"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="21"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="21"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="21"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="21"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="21"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="21"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="21"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="21"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="21"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="21"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="21"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="21"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="21"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="21"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="21"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="21"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="21"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="21"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="21"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="21"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="21"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="21"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="21"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="21"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="21"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="21"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="21"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="21"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="21"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="21"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="21"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="21"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="21"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="21"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="21"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="21"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="21"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="21"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="21"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="21"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="21"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="21"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="21"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="21"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="21"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="21"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="21"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="21"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="21"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="21"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="21"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="21"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="21"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="21"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="21"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="21"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="21"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="21"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="21"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="21"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="21"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="21"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="21"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="21"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="21"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="21"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="21"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="21"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="21"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="21"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="21"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="21"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="21"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="21"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="21"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="21"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="21"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="21"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="21"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="21"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="21"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="21"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="21"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="21"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="21"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="21"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="21"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="21"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="21"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="21"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="21"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="21"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="21"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="21"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="21"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="21"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="21"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="21"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="21"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="21"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="21"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="21"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="21"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="21"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="21"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="21"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="21"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="21"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="21"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="21"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="21"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="21"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="21"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="21"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="21"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="21"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="21"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="21"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="21"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="21"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="21"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="21"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="21"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="21"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="21"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="21"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="21"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="21"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="21"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="21"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="21"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="21"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="21"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="21"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="21"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="21"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="21"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="21"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="21"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="21"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="21"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="21"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="21"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="21"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="21"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="21"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="21"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="21"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="21"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="21"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="21"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="21"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="21"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="21"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="21"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="21"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="21"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="21"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="21"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="21"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="21"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="21"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="21"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="21"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="21"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="21"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="21"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="21"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="21"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="21"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="21"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="21"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="21"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="21"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="21"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="21"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="21"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="21"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="21"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="21"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="21"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="21"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="21"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="21"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="21"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="21"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="21"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="21"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="21"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="21"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="21"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="21"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="21"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="21"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="21"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="21"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="21"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="21"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="21"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="21"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="21"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="21"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="21"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="21"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="21"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="21"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="21"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="21"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="21"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="21"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="21"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="21"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="21"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="21"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="21"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="21"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="21"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="21"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="21"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="21"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="21"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="21"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="21"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="21"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="21"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="21"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="21"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="21"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="21"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="21"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="21"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="21"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="21"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="21"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="21"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="21"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="21"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="21"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="21"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="21"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="21"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="21"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="21"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="21"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="21"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="21"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
change in feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -117,6 +117,12 @@
     <t>InvalidDate</t>
   </si>
   <si>
+    <t>validweight_overweight</t>
+  </si>
+  <si>
+    <t>validheight_overweight</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -245,37 +251,71 @@
 Vitamin D, Insulin</t>
   </si>
   <si>
+    <t>Free Plan</t>
+  </si>
+  <si>
+    <t>User2@gmail.com</t>
+  </si>
+  <si>
+    <t>User2*/245</t>
+  </si>
+  <si>
+    <t>PCOS</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>I'm not sure</t>
+  </si>
+  <si>
+    <t>My cycle is irregular</t>
+  </si>
+  <si>
+    <t>Vegetarian Diet</t>
+  </si>
+  <si>
+    <t>Sedentary</t>
+  </si>
+  <si>
+    <t>No, I can eat everything</t>
+  </si>
+  <si>
+    <t>No, I don't take any medications or supplements</t>
+  </si>
+  <si>
     <t>Free</t>
   </si>
   <si>
-    <t>User2@gmail.com</t>
-  </si>
-  <si>
-    <t>User2*/245</t>
-  </si>
-  <si>
-    <t>PCOS</t>
-  </si>
-  <si>
-    <t>User2</t>
-  </si>
-  <si>
-    <t>I'm not sure</t>
-  </si>
-  <si>
-    <t>My cycle is irregular</t>
-  </si>
-  <si>
-    <t>Vegetarian Diet</t>
-  </si>
-  <si>
-    <t>Sedentary</t>
-  </si>
-  <si>
-    <t>No, I can eat everything</t>
-  </si>
-  <si>
-    <t>No, I don't take any medications or supplements</t>
+    <t>User_WithoutReport_WithOnlyHealthCondition</t>
+  </si>
+  <si>
+    <t>gurdev@gmail.com</t>
+  </si>
+  <si>
+    <t>Success@1</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>gurdev</t>
+  </si>
+  <si>
+    <t>I have never been diagnosed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Non-Vegetarian</t>
+  </si>
+  <si>
+    <t>User_WithoutReport_WithoutHealthCondition</t>
+  </si>
+  <si>
+    <t>dheena@gmail.com</t>
+  </si>
+  <si>
+    <t>dheena</t>
   </si>
 </sst>
 </file>
@@ -374,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -392,6 +432,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -423,14 +466,23 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,25 +855,37 @@
       <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>34.0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>170.0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>0.0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>-4.0</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>46036.0</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>45143.0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>170.0</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +925,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -872,10 +936,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -883,18 +947,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1927,18 +1991,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1957,199 +2021,3263 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="L1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
+      <c r="R1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="14">
+      <c r="E2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="15">
         <v>43.0</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="H2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="16">
         <v>46031.0</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="15">
         <v>67.0</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="15">
         <v>145.0</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="15">
+        <v>25.0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="16">
+        <v>46054.0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>160.0</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="19"/>
+      <c r="S3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="J4" s="21">
+        <v>46036.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>155.0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="O4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="14">
-        <v>25.0</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="15">
-        <v>46054.0</v>
-      </c>
-      <c r="K3" s="14">
-        <v>56.0</v>
-      </c>
-      <c r="L3" s="14">
-        <v>160.0</v>
-      </c>
-      <c r="M3" s="13" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="18"/>
-      <c r="S3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
+      <c r="I5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="22"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="22"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="22"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="22"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="22"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="22"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="22"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="22"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="22"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="22"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="22"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="22"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="22"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="22"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="22"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="22"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="22"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="22"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="22"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="22"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="22"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="22"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="22"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="22"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="22"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="22"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="22"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="22"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="22"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="22"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="22"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="22"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="22"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="22"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="22"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="22"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="22"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="22"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="22"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="22"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="22"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="22"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="22"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="22"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="22"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="22"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="22"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="22"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="22"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="22"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="22"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="22"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="22"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="22"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="22"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="22"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="22"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="22"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="22"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="22"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="22"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="22"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="22"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="22"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="22"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="22"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="22"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="22"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="22"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="22"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="22"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="22"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="22"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="22"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="22"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="22"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="22"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="22"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="22"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="22"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="22"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="22"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="22"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="22"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="22"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="22"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="22"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="22"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="22"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="22"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="22"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="22"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="22"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="22"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="22"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="22"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="22"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="22"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="22"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="22"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="22"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="22"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="22"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="22"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="22"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="22"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="22"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="22"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="22"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="22"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="22"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="22"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="22"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="22"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="22"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="22"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="22"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="22"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="22"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="22"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="22"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="22"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="22"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="22"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="22"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="22"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="22"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="22"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="22"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="22"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="22"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="22"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="22"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="22"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="22"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="22"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="22"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="22"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="22"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="22"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="22"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="22"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="22"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="22"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="22"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="22"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="22"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="22"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="22"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="22"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="22"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="22"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="22"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="22"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="22"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="22"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="22"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="22"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="22"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="22"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="22"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="22"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="22"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="22"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="22"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="22"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="22"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="22"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="22"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="22"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="22"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="22"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="22"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="22"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="22"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="22"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="22"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="22"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="22"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="22"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="22"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="22"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="22"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="22"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="22"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="22"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="22"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="22"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="22"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="22"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="22"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="22"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="22"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="22"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="22"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="22"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="22"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="22"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="22"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="22"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="22"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="22"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="22"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="22"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="22"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="22"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="22"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="22"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="22"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="22"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="22"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="22"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="22"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="22"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="22"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="22"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="22"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="22"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="22"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="22"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="22"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="22"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="22"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="22"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="22"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="22"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="22"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="22"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="22"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="22"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="22"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="22"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="22"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="22"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="22"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="22"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="22"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="22"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="22"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="22"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="22"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="22"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="22"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="22"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="22"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="22"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="22"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="22"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="22"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="22"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="22"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="22"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="22"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="22"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="22"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="22"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="22"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="22"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="22"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="22"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="22"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="22"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="22"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="22"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="22"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="22"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="22"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="22"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="22"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="22"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="22"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="22"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="22"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="22"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="22"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="22"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="22"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="22"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="22"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="22"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="22"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="22"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="22"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="22"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="22"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="22"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="22"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="22"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="22"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="22"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="22"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="22"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="22"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="22"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="22"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="22"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="22"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="22"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="22"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="22"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="22"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="22"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="22"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="22"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="22"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="22"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="22"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="22"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="22"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="22"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="22"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="22"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="22"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="22"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="22"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="22"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="22"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="22"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="22"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="22"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="22"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="22"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="22"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="22"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="22"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="22"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="22"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="22"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="22"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="22"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="22"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="22"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="22"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="22"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="22"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="22"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="22"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="22"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="22"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="22"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="22"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="22"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="22"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="22"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="22"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="22"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="22"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="22"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="22"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="22"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="22"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="22"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="22"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="22"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="22"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="22"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="22"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="22"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="22"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="22"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="22"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="22"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="22"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="22"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="22"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="22"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="22"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="22"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="22"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="22"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="22"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="22"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="22"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="22"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="22"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="22"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="22"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="22"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="22"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="22"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="22"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="22"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="22"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="22"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="22"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="22"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="22"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="22"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="22"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="22"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="22"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="22"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="22"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="22"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="22"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="22"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="22"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="22"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="22"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="22"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="22"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="22"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="22"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="22"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="22"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="22"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="22"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="22"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="22"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="22"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="22"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="22"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="22"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="22"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="22"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="22"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="22"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="22"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="22"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="22"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="22"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="22"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="22"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="22"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="22"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="22"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="22"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="22"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="22"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="22"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="22"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="22"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="22"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="22"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="22"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="22"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="22"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="22"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="22"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="22"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="22"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="22"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="22"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="22"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="22"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="22"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="22"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="22"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="22"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="22"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="22"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="22"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="22"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="22"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="22"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="22"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="22"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="22"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="22"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="22"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="22"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="22"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="22"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="22"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="22"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="22"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="22"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="22"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="22"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="22"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="22"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="22"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="22"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="22"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="22"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="22"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="22"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="22"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="22"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="22"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="22"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="22"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="22"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="22"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="22"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="22"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="22"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="22"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="22"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="22"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="22"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="22"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="22"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="22"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="22"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="22"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="22"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="22"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="22"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="22"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="22"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="22"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="22"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="22"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="22"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="22"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="22"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="22"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="22"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="22"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="22"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="22"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="22"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="22"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="22"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="22"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="22"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="22"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="22"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="22"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="22"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="22"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="22"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="22"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="22"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="22"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="22"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="22"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="22"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="22"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="22"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="22"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="22"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="22"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="22"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="22"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="22"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="22"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="22"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="22"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="22"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="22"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="22"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="22"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="22"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="22"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="22"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="22"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="22"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="22"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="22"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="22"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="22"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="22"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="22"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="22"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="22"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="22"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="22"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="22"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="22"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="22"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="22"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="22"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="22"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="22"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="22"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="22"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="22"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="22"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="22"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="22"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="22"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="22"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="22"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="22"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="22"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="22"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="22"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="22"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="22"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="22"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="22"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="22"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="22"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="22"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="22"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="22"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="22"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="22"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="22"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="22"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="22"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="22"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="22"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="22"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="22"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="22"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="22"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="22"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="22"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="22"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="22"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="22"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="22"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="22"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="22"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="22"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="22"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="22"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="22"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="22"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="22"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="22"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="22"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="22"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="22"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="22"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="22"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="22"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="22"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="22"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="22"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="22"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="22"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="22"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="22"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="22"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="22"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="22"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="22"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="22"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="22"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="22"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="22"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="22"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="22"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="22"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="22"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="22"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="22"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="22"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="22"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="22"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="22"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="22"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="22"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="22"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="22"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="22"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="22"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="22"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="22"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="22"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="22"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="22"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="22"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="22"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="22"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="22"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="22"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="22"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="22"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="22"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="22"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="22"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="22"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="22"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="22"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="22"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="22"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="22"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="22"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="22"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="22"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="22"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="22"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="22"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="22"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="22"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="22"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="22"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="22"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="22"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="22"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="22"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="22"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="22"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="22"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="22"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="22"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="22"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="22"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="22"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="22"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="22"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="22"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="22"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="22"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="22"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="22"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="22"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="22"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="22"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="22"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="22"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="22"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="22"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="22"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="22"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="22"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="22"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="22"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="22"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="22"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="22"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="22"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="22"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="22"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="22"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="22"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="22"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="22"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="22"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="22"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="22"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="22"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="22"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="22"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="22"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="22"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="22"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="22"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="22"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="22"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="22"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="22"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="22"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="22"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="22"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="22"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="22"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="22"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="22"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="22"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="22"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="22"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="22"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="22"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="22"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="22"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="22"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="22"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="22"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="22"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="22"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="22"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="22"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="22"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="22"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="22"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="22"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="22"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="22"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="22"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="22"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="22"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="22"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="22"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="22"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="22"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="22"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="22"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="22"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="22"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="22"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="22"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="22"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="22"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="22"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="22"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="22"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="22"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="22"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="22"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="22"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="22"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="22"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="22"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="22"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="22"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="22"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="22"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="22"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="22"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="22"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="22"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="22"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="22"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="22"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="22"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="22"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="22"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="22"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="22"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="22"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="22"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="22"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="22"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="22"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="22"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="22"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="22"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="22"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="22"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="22"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="22"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="22"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="22"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="22"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="22"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="22"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="22"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="22"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="22"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="22"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="22"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="22"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="22"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="22"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="22"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="22"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="22"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="22"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="22"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="22"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="22"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="22"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="22"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="22"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="22"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="22"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="22"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="22"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="22"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="22"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="22"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="22"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="22"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="22"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="22"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="22"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="22"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="22"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="22"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="22"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="22"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="22"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="22"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="22"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="22"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="22"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="22"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="22"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="22"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="22"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="22"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="22"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="22"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="22"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="22"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="22"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="22"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="22"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="22"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="22"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="22"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="22"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="22"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="22"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="22"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="22"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="22"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="22"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="22"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="22"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="22"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="22"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="22"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="22"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="22"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="22"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="22"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="22"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="22"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="22"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="22"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="22"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="22"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="22"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="22"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="22"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="22"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="22"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="22"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="22"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="22"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="22"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="22"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="22"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="22"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="22"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="22"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="22"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="22"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="22"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="22"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="22"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="22"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="22"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="22"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="22"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="22"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="22"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="22"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="22"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="22"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="22"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="22"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="22"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="22"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="22"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="22"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="22"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="22"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="22"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="22"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="22"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="22"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="22"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="22"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="22"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="22"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="22"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="22"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="22"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="22"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="22"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="22"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="22"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="22"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="22"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="22"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="22"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="22"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="22"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="22"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="22"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="22"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="22"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="22"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="22"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
few dashboard features completed
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -15,14 +15,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="25EM24IIZ0N63hnweokl8H6zL72aFDhrpFxfveJYOlI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataChecksum="t4f85315oZeYzB3iR8O3SlURAbhmYgzYUSDhuhPWuK8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -117,6 +117,12 @@
     <t>InvalidDate</t>
   </si>
   <si>
+    <t>validweight_overweight</t>
+  </si>
+  <si>
+    <t>validheight_overweight</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -202,6 +208,9 @@
     <t>Plan</t>
   </si>
   <si>
+    <t>User_WithoutReport</t>
+  </si>
+  <si>
     <t>User1@gmail.com</t>
   </si>
   <si>
@@ -242,37 +251,71 @@
 Vitamin D, Insulin</t>
   </si>
   <si>
+    <t>Free Plan</t>
+  </si>
+  <si>
+    <t>User2@gmail.com</t>
+  </si>
+  <si>
+    <t>User2*/245</t>
+  </si>
+  <si>
+    <t>PCOS</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>I'm not sure</t>
+  </si>
+  <si>
+    <t>My cycle is irregular</t>
+  </si>
+  <si>
+    <t>Vegetarian Diet</t>
+  </si>
+  <si>
+    <t>Sedentary</t>
+  </si>
+  <si>
+    <t>No, I can eat everything</t>
+  </si>
+  <si>
+    <t>No, I don't take any medications or supplements</t>
+  </si>
+  <si>
     <t>Free</t>
   </si>
   <si>
-    <t>User2@gmail.com</t>
-  </si>
-  <si>
-    <t>User2*/245</t>
-  </si>
-  <si>
-    <t>PCOS</t>
-  </si>
-  <si>
-    <t>User2</t>
-  </si>
-  <si>
-    <t>I'm not sure</t>
-  </si>
-  <si>
-    <t>My cycle is irregular</t>
-  </si>
-  <si>
-    <t>Vegetarian Diet</t>
-  </si>
-  <si>
-    <t>Sedentary</t>
-  </si>
-  <si>
-    <t>No, I can eat everything</t>
-  </si>
-  <si>
-    <t>No, I don't take any medications or supplements</t>
+    <t>User_WithoutReport_WithOnlyHealthCondition</t>
+  </si>
+  <si>
+    <t>gurdev@gmail.com</t>
+  </si>
+  <si>
+    <t>Success@1</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>gurdev</t>
+  </si>
+  <si>
+    <t>I have never been diagnosed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Non-Vegetarian</t>
+  </si>
+  <si>
+    <t>User_WithoutReport_WithoutHealthCondition</t>
+  </si>
+  <si>
+    <t>dheena@gmail.com</t>
+  </si>
+  <si>
+    <t>dheena</t>
   </si>
 </sst>
 </file>
@@ -371,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -391,6 +434,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -399,11 +445,17 @@
     <xf borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -414,11 +466,23 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,25 +855,37 @@
       <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>34.0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>170.0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>0.0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>-4.0</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>46036.0</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>45143.0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>170.0</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +925,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -860,10 +936,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -871,18 +947,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1915,18 +1991,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1945,192 +2021,3263 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="Q1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="R1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="12">
+      <c r="D2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="15">
         <v>43.0</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="16">
+        <v>46031.0</v>
+      </c>
+      <c r="K2" s="15">
+        <v>67.0</v>
+      </c>
+      <c r="L2" s="15">
+        <v>145.0</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="13">
-        <v>46031.0</v>
-      </c>
-      <c r="J2" s="12">
-        <v>67.0</v>
-      </c>
-      <c r="K2" s="12">
-        <v>145.0</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="E3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="15">
+        <v>25.0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="16">
+        <v>46054.0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>160.0</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="19"/>
+      <c r="S3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="11" t="s">
+      <c r="J4" s="21">
+        <v>46036.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>155.0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="O4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="12">
-        <v>25.0</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="13">
-        <v>46054.0</v>
-      </c>
-      <c r="J3" s="12">
-        <v>56.0</v>
-      </c>
-      <c r="K3" s="12">
-        <v>160.0</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="11" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
+      <c r="I5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="22"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="22"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="22"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="22"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="22"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="22"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="22"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="22"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="22"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="22"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="22"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="22"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="22"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="22"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="22"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="22"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="22"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="22"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="22"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="22"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="22"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="22"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="22"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="22"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="22"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="22"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="22"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="22"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="22"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="22"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="22"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="22"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="22"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="22"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="22"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="22"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="22"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="22"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="22"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="22"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="22"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="22"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="22"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="22"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="22"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="22"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="22"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="22"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="22"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="22"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="22"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="22"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="22"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="22"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="22"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="22"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="22"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="22"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="22"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="22"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="22"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="22"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="22"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="22"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="22"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="22"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="22"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="22"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="22"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="22"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="22"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="22"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="22"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="22"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="22"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="22"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="22"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="22"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="22"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="22"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="22"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="22"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="22"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="22"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="22"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="22"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="22"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="22"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="22"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="22"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="22"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="22"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="22"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="22"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="22"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="22"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="22"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="22"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="22"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="22"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="22"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="22"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="22"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="22"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="22"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="22"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="22"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="22"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="22"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="22"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="22"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="22"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="22"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="22"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="22"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="22"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="22"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="22"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="22"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="22"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="22"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="22"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="22"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="22"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="22"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="22"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="22"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="22"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="22"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="22"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="22"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="22"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="22"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="22"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="22"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="22"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="22"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="22"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="22"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="22"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="22"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="22"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="22"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="22"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="22"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="22"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="22"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="22"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="22"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="22"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="22"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="22"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="22"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="22"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="22"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="22"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="22"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="22"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="22"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="22"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="22"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="22"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="22"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="22"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="22"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="22"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="22"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="22"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="22"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="22"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="22"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="22"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="22"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="22"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="22"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="22"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="22"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="22"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="22"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="22"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="22"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="22"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="22"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="22"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="22"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="22"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="22"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="22"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="22"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="22"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="22"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="22"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="22"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="22"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="22"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="22"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="22"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="22"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="22"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="22"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="22"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="22"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="22"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="22"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="22"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="22"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="22"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="22"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="22"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="22"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="22"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="22"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="22"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="22"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="22"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="22"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="22"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="22"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="22"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="22"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="22"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="22"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="22"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="22"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="22"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="22"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="22"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="22"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="22"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="22"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="22"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="22"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="22"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="22"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="22"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="22"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="22"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="22"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="22"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="22"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="22"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="22"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="22"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="22"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="22"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="22"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="22"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="22"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="22"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="22"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="22"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="22"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="22"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="22"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="22"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="22"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="22"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="22"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="22"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="22"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="22"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="22"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="22"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="22"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="22"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="22"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="22"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="22"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="22"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="22"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="22"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="22"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="22"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="22"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="22"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="22"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="22"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="22"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="22"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="22"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="22"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="22"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="22"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="22"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="22"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="22"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="22"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="22"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="22"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="22"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="22"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="22"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="22"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="22"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="22"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="22"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="22"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="22"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="22"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="22"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="22"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="22"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="22"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="22"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="22"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="22"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="22"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="22"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="22"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="22"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="22"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="22"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="22"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="22"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="22"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="22"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="22"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="22"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="22"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="22"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="22"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="22"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="22"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="22"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="22"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="22"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="22"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="22"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="22"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="22"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="22"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="22"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="22"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="22"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="22"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="22"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="22"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="22"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="22"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="22"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="22"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="22"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="22"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="22"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="22"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="22"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="22"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="22"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="22"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="22"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="22"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="22"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="22"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="22"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="22"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="22"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="22"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="22"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="22"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="22"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="22"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="22"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="22"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="22"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="22"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="22"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="22"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="22"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="22"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="22"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="22"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="22"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="22"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="22"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="22"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="22"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="22"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="22"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="22"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="22"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="22"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="22"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="22"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="22"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="22"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="22"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="22"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="22"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="22"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="22"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="22"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="22"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="22"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="22"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="22"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="22"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="22"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="22"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="22"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="22"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="22"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="22"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="22"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="22"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="22"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="22"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="22"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="22"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="22"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="22"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="22"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="22"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="22"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="22"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="22"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="22"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="22"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="22"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="22"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="22"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="22"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="22"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="22"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="22"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="22"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="22"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="22"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="22"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="22"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="22"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="22"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="22"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="22"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="22"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="22"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="22"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="22"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="22"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="22"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="22"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="22"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="22"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="22"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="22"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="22"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="22"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="22"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="22"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="22"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="22"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="22"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="22"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="22"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="22"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="22"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="22"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="22"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="22"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="22"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="22"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="22"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="22"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="22"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="22"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="22"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="22"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="22"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="22"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="22"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="22"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="22"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="22"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="22"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="22"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="22"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="22"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="22"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="22"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="22"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="22"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="22"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="22"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="22"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="22"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="22"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="22"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="22"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="22"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="22"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="22"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="22"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="22"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="22"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="22"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="22"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="22"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="22"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="22"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="22"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="22"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="22"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="22"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="22"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="22"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="22"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="22"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="22"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="22"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="22"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="22"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="22"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="22"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="22"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="22"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="22"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="22"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="22"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="22"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="22"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="22"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="22"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="22"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="22"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="22"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="22"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="22"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="22"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="22"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="22"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="22"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="22"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="22"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="22"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="22"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="22"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="22"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="22"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="22"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="22"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="22"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="22"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="22"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="22"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="22"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="22"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="22"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="22"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="22"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="22"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="22"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="22"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="22"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="22"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="22"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="22"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="22"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="22"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="22"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="22"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="22"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="22"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="22"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="22"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="22"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="22"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="22"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="22"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="22"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="22"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="22"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="22"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="22"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="22"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="22"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="22"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="22"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="22"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="22"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="22"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="22"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="22"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="22"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="22"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="22"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="22"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="22"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="22"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="22"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="22"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="22"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="22"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="22"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="22"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="22"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="22"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="22"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="22"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="22"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="22"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="22"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="22"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="22"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="22"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="22"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="22"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="22"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="22"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="22"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="22"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="22"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="22"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="22"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="22"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="22"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="22"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="22"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="22"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="22"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="22"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="22"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="22"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="22"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="22"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="22"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="22"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="22"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="22"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="22"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="22"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="22"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="22"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="22"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="22"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="22"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="22"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="22"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="22"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="22"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="22"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="22"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="22"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="22"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="22"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="22"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="22"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="22"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="22"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="22"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="22"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="22"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="22"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="22"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="22"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="22"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="22"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="22"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="22"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="22"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="22"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="22"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="22"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="22"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="22"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="22"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="22"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="22"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="22"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="22"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="22"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="22"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="22"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="22"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="22"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="22"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="22"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="22"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="22"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="22"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="22"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="22"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="22"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="22"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="22"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="22"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="22"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="22"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="22"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="22"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="22"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="22"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="22"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="22"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="22"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="22"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="22"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="22"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="22"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="22"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="22"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="22"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="22"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="22"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="22"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="22"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="22"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="22"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="22"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="22"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="22"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="22"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="22"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="22"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="22"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="22"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="22"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="22"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="22"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="22"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="22"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="22"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="22"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="22"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="22"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="22"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="22"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="22"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="22"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="22"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="22"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="22"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="22"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="22"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="22"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="22"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="22"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="22"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="22"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="22"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="22"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="22"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="22"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="22"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="22"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="22"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="22"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="22"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="22"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="22"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="22"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="22"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="22"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="22"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="22"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="22"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="22"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="22"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="22"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="22"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="22"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="22"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="22"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="22"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="22"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="22"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="22"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="22"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="22"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="22"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="22"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="22"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="22"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="22"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="22"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="22"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="22"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="22"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="22"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="22"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="22"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="22"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="22"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="22"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="22"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="22"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="22"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="22"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="22"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="22"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="22"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="22"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="22"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="22"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="22"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="22"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="22"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="22"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="22"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="22"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="22"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="22"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="22"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="22"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="22"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="22"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="22"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="22"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="22"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="22"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="22"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="22"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="22"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="22"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="22"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="22"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="22"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="22"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="22"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="22"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="22"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="22"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="22"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="22"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="22"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="22"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="22"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="22"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="22"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="22"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="22"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="22"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="22"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="22"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="22"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="22"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="22"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="22"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="22"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="22"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="22"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="22"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="22"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="22"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="22"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="22"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="22"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="22"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="22"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="22"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="22"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="22"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="22"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="22"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="22"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="22"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="22"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="22"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="22"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="22"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="22"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="22"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="22"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="22"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="22"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="22"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="22"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="22"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="22"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="22"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="22"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="22"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="22"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="22"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="22"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="22"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="22"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="22"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="22"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="22"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="22"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="22"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="22"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="22"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="22"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="22"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="22"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="22"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="22"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="22"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="22"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="22"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="22"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="22"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="22"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="22"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="22"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="22"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="22"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="22"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="22"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="22"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="22"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="22"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="22"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="22"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="22"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="22"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="22"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="22"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="22"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="22"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="22"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="22"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="22"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="22"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="22"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="22"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="22"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="22"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="22"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="22"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="22"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="22"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="22"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="22"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="22"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="22"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="22"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="22"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="22"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="22"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="22"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="22"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="22"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="22"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="22"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="22"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="22"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="22"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="22"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="22"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="22"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="22"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="22"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="22"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="22"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="22"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="22"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="22"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="22"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="22"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="22"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="22"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="22"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="22"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="22"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="22"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="22"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="22"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="22"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="22"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="22"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="22"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Creating step def for OnBoarding Step 5
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
+++ b/src/test/resources/TestData/Team01_Selenium_Titans_TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -117,6 +117,12 @@
     <t>InvalidDate</t>
   </si>
   <si>
+    <t>validweight_overweight</t>
+  </si>
+  <si>
+    <t>validheight_overweight</t>
+  </si>
+  <si>
     <t>Scenario</t>
   </si>
   <si>
@@ -279,6 +285,37 @@
   </si>
   <si>
     <t>Free</t>
+  </si>
+  <si>
+    <t>User_WithoutReport_WithOnlyHealthCondition</t>
+  </si>
+  <si>
+    <t>gurdev@gmail.com</t>
+  </si>
+  <si>
+    <t>Success@1</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>gurdev</t>
+  </si>
+  <si>
+    <t>I have never been diagnosed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Non-Vegetarian</t>
+  </si>
+  <si>
+    <t>User_WithoutReport_WithoutHealthCondition</t>
+  </si>
+  <si>
+    <t>dheena@gmail.com</t>
+  </si>
+  <si>
+    <t>dheena</t>
   </si>
 </sst>
 </file>
@@ -377,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -395,6 +432,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -432,11 +472,17 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,25 +855,37 @@
       <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>34.0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>170.0</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>0.0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>-4.0</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <v>46036.0</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>45143.0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>80.0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>170.0</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +925,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -878,10 +936,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -889,18 +947,18 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1"/>
@@ -1933,18 +1991,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1963,199 +2021,3263 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="L1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
+      <c r="R1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="14">
+      <c r="E2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="15">
         <v>43.0</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="H2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="16">
         <v>46031.0</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="15">
         <v>67.0</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="15">
         <v>145.0</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="15">
+        <v>25.0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="16">
+        <v>46054.0</v>
+      </c>
+      <c r="K3" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="L3" s="15">
+        <v>160.0</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="19"/>
+      <c r="S3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="J4" s="21">
+        <v>46036.0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>155.0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="O4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="14">
-        <v>25.0</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="15">
-        <v>46054.0</v>
-      </c>
-      <c r="K3" s="14">
-        <v>56.0</v>
-      </c>
-      <c r="L3" s="14">
-        <v>160.0</v>
-      </c>
-      <c r="M3" s="13" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
+      <c r="I5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="22"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="22"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="22"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="22"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="22"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="22"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="22"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="22"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="22"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="22"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="22"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="22"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="22"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="22"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="22"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="22"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="22"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="22"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="22"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="22"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="22"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="22"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="22"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="22"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="22"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="22"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="22"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="22"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="22"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="22"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="22"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="22"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="22"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="22"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="22"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="22"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="22"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="22"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="22"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="22"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="22"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="22"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="22"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="22"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="22"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="22"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="22"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="22"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="22"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="22"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="22"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="22"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="22"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="22"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="22"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="22"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="22"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="22"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="22"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="22"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="22"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="22"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="22"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="22"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="22"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="22"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="22"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="22"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="22"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="22"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="22"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="22"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="22"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="22"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="22"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="22"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="22"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="22"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="22"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="22"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="22"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="22"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="22"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="22"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="22"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="22"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="22"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="22"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="22"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="22"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="22"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="22"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="22"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="22"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="22"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="22"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="22"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="22"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="22"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="22"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="22"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="22"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="22"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="22"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="22"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="22"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="22"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="22"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="22"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="22"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="22"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="22"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="22"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="22"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="22"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="22"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="22"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="22"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="22"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="22"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="22"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="22"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="22"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="22"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="22"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="22"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="22"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="22"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="22"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="22"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="22"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="22"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="22"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="22"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="22"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="22"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="22"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="22"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="22"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="22"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="22"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="22"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="22"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="22"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="22"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="22"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="22"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="22"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="22"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="22"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="22"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="22"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="22"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="22"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="22"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="22"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="22"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="22"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="22"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="22"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="22"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="22"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="22"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="22"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="22"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="22"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="22"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="22"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="22"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="22"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="22"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="22"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="22"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="22"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="22"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="22"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="22"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="22"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="22"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="22"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="22"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="22"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="22"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="22"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="22"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="22"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="22"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="22"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="22"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="22"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="22"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="22"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="22"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="22"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="22"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="22"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="22"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="22"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="22"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="22"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="22"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="22"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="22"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="22"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="22"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="22"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="22"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="22"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="22"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="22"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="22"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="22"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="22"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="22"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="22"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="22"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="22"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="22"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="22"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="22"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="22"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="22"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="22"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="22"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="22"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="22"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="22"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="22"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="22"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="22"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="22"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="22"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="22"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="22"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="22"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="22"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="22"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="22"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="22"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="22"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="22"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="22"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="22"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="22"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="22"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="22"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="22"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="22"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="22"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="22"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="22"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="22"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="22"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="22"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="22"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="22"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="22"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="22"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="22"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="22"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="22"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="22"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="22"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="22"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="22"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="22"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="22"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="22"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="22"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="22"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="22"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="22"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="22"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="22"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="22"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="22"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="22"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="22"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="22"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="22"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="22"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="22"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="22"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="22"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="22"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="22"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="22"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="22"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="22"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="22"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="22"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="22"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="22"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="22"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="22"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="22"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="22"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="22"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="22"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="22"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="22"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="22"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="22"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="22"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="22"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="22"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="22"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="22"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="22"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="22"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="22"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="22"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="22"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="22"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="22"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="22"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="22"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="22"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="22"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="22"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="22"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="22"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="22"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="22"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="22"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="22"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="22"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="22"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="22"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="22"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="22"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="22"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="22"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="22"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="22"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="22"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="22"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="22"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="22"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="22"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="22"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="22"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="22"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="22"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="22"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="22"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="22"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="22"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="22"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="22"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="22"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="22"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="22"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="22"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="22"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="22"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="22"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="22"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="22"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="22"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="22"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="22"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="22"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="22"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="22"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="22"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="22"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="22"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="22"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="22"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="22"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="22"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="22"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="22"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="22"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="22"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="22"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="22"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="22"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="22"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="22"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="22"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="22"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="22"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="22"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="22"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="22"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="22"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="22"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="22"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="22"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="22"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="22"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="22"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="22"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="22"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="22"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="22"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="22"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="22"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="22"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="22"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="22"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="22"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="22"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="22"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="22"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="22"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="22"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="22"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="22"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="22"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="22"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="22"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="22"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="22"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="22"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="22"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="22"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="22"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="22"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="22"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="22"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="22"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="22"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="22"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="22"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="22"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="22"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="22"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="22"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="22"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="22"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="22"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="22"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="22"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="22"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="22"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="22"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="22"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="22"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="22"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="22"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="22"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="22"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="22"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="22"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="22"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="22"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="22"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="22"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="22"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="22"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="22"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="22"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="22"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="22"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="22"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="22"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="22"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="22"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="22"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="22"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="22"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="22"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="22"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="22"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="22"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="22"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="22"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="22"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="22"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="22"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="22"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="22"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="22"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="22"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="22"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="22"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="22"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="22"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="22"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="22"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="22"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="22"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="22"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="22"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="22"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="22"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="22"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="22"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="22"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="22"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="22"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="22"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="22"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="22"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="22"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="22"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="22"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="22"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="22"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="22"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="22"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="22"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="22"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="22"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="22"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="22"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="22"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="22"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="22"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="22"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="22"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="22"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="22"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="22"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="22"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="22"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="22"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="22"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="22"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="22"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="22"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="22"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="22"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="22"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="22"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="22"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="22"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="22"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="22"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="22"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="22"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="22"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="22"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="22"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="22"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="22"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="22"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="22"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="22"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="22"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="22"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="22"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="22"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="22"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="22"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="22"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="22"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="22"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="22"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="22"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="22"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="22"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="22"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="22"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="22"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="22"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="22"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="22"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="22"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="22"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="22"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="22"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="22"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="22"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="22"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="22"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="22"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="22"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="22"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="22"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="22"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="22"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="22"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="22"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="22"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="22"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="22"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="22"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="22"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="22"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="22"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="22"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="22"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="22"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="22"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="22"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="22"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="22"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="22"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="22"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="22"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="22"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="22"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="22"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="22"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="22"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="22"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="22"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="22"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="22"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="22"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="22"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="22"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="22"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="22"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="22"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="22"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="22"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="22"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="22"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="22"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="22"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="22"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="22"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="22"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="22"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="22"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="22"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="22"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="22"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="22"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="22"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="22"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="22"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="22"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="22"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="22"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="22"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="22"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="22"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="22"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="22"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="22"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="22"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="22"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="22"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="22"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="22"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="22"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="22"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="22"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="22"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="22"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="22"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="22"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="22"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="22"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="22"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="22"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="22"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="22"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="22"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="22"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="22"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="22"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="22"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="22"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="22"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="22"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="22"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="22"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="22"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="22"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="22"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="22"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="22"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="22"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="22"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="22"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="22"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="22"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="22"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="22"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="22"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="22"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="22"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="22"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="22"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="22"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="22"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="22"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="22"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="22"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="22"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="22"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="22"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="22"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="22"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="22"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="22"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="22"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="22"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="22"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="22"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="22"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="22"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="22"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="22"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="22"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="22"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="22"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="22"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="22"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="22"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="22"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="22"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="22"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="22"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="22"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="22"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="22"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="22"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="22"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="22"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="22"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="22"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="22"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="22"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="22"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="22"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="22"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="22"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="22"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="22"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="22"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="22"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="22"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="22"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="22"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="22"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="22"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="22"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="22"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="22"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="22"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="22"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="22"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="22"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="22"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="22"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="22"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="22"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="22"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="22"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="22"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="22"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="22"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="22"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="22"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="22"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="22"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="22"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="22"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="22"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="22"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="22"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="22"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="22"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="22"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="22"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="22"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="22"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="22"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="22"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="22"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="22"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="22"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="22"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="22"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="22"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="22"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="22"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="22"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="22"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="22"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="22"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="22"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="22"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="22"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="22"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="22"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="22"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="22"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="22"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="22"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="22"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="22"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="22"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="22"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="22"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="22"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="22"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="22"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="22"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="22"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="22"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="22"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="22"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="22"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="22"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="22"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="22"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="22"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="22"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="22"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="22"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="22"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="22"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="22"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="22"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="22"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="22"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="22"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="22"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="22"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="22"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="22"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="22"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="22"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="22"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="22"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="22"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="22"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="22"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="22"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="22"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="22"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="22"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="22"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="22"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="22"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="22"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="22"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="22"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="22"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="22"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="22"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="22"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="22"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="22"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="22"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="22"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="22"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="22"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="22"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="22"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="22"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="22"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="22"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="22"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="22"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="22"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="22"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="22"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="22"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="22"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="22"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="22"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="22"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="22"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="22"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="22"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="22"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="22"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="22"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="22"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="22"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="22"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="22"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="22"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="22"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="22"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="22"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="22"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="22"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="22"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="22"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="22"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="22"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="22"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="22"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="22"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="22"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="22"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="22"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="22"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="22"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="22"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="22"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="22"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="22"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="22"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="22"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="22"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="22"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="22"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="22"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="22"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="22"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="22"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="22"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="22"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="22"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="22"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="22"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="22"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="22"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="22"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="22"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="22"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="22"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="22"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="22"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="22"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="22"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="22"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="22"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="22"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="22"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="22"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="22"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="22"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="22"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="22"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="22"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="22"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="22"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="22"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="22"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="22"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="22"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="22"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="22"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="22"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="22"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="22"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="22"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="22"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="22"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="22"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="22"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="22"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="22"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="22"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="22"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="22"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="22"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="22"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="22"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="22"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="22"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="22"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="22"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="22"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="22"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="22"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="22"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="22"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="22"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="22"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="22"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="22"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="22"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="22"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="22"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="22"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>